<commit_message>
In progress Data Preparation
</commit_message>
<xml_diff>
--- a/tblReport Query.xlsx
+++ b/tblReport Query.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\424792\Documents\Work\Data Repository\Portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db0c9f1a5e8d4b91/Documents/zzDocuments/Git_TJ_Portfolio/Projct1-Python-docx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D5AD5C-58EE-4C54-8920-E20520D88499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{40D5AD5C-58EE-4C54-8920-E20520D88499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67E74D9B-E61D-45DC-BC11-7383E81334E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-645" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tblReport Query" sheetId="1" r:id="rId1"/>
@@ -382,30 +382,30 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,19 +749,24 @@
   <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="45.140625" customWidth="1"/>
-    <col min="13" max="13" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2862,7 +2867,7 @@
         <v>44834</v>
       </c>
       <c r="L66" s="5" t="str">
-        <f t="shared" ref="L66:L97" si="2">B66&amp;" "&amp;C66&amp;"-"&amp;M66&amp;" Action Details"</f>
+        <f t="shared" ref="L66:L86" si="2">B66&amp;" "&amp;C66&amp;"-"&amp;M66&amp;" Action Details"</f>
         <v>Management Controls 1-65 Action Details</v>
       </c>
       <c r="M66" s="8">

</xml_diff>